<commit_message>
Clean Up, Improved Test Coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/lodicity.schema.xlsx
+++ b/src/test/resources/lodicity.schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DataObject" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Attribute</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>SimpleType</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -179,14 +191,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -290,6 +302,28 @@
         <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -311,7 +345,7 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
82,5 % Test Coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/lodicity.schema.xlsx
+++ b/src/test/resources/lodicity.schema.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DataObject" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SimpleType" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="StrictType" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Attribute</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>musthavestring</t>
   </si>
 </sst>
 </file>
@@ -191,14 +195,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -327,6 +331,7 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -410,4 +415,60 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>